<commit_message>
Added unit testing for Game.CheckSOS
</commit_message>
<xml_diff>
--- a/artifacts/sprint-3-logs.xlsx
+++ b/artifacts/sprint-3-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41B8397-B7C9-4DAC-99C2-F3CA46883C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2845AF9-125D-46FD-84E2-470DDAB14965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16290" yWindow="-10785" windowWidth="16410" windowHeight="11295" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16290" yWindow="-10785" windowWidth="16410" windowHeight="11295" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="399">
   <si>
     <t>ID</t>
   </si>
@@ -1275,6 +1275,51 @@
   </si>
   <si>
     <t>It is still the red player's turn</t>
+  </si>
+  <si>
+    <t>SOS line (last O) -&gt;vertical line case</t>
+  </si>
+  <si>
+    <t>SOS line (last O) -&gt;horizontal line case</t>
+  </si>
+  <si>
+    <t>SOS line (last O) -&gt; positive diagonal case</t>
+  </si>
+  <si>
+    <t>SOS line (last O) -&gt; negative diagonal case</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; vertical line case (last move on top S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; vertical line case (last move on bottom S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; horizontal line case (last move on right S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; horizontal line case (last move on left S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; positive diagonal case (last move on top-right S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; positive diagonal case (last move on bottom-left S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; negative diagonal case (last move on top-left S)</t>
+  </si>
+  <si>
+    <t>SOS line (last S) -&gt; negative diagonal case (last move on bottom-right S)</t>
+  </si>
+  <si>
+    <t>Game.CheckSOS</t>
+  </si>
+  <si>
+    <t>Game.TestCheckSOS</t>
+  </si>
+  <si>
+    <t>New SOS line appended to Game.sosLines</t>
   </si>
 </sst>
 </file>
@@ -1695,8 +1740,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="B2:F16" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}" name="Table9" displayName="Table9" ref="B2:F28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="B2:F28" xr:uid="{0F699053-0EA0-422C-84BA-6343D3283560}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7EE5C09C-96A5-4FC0-A9B8-78BA2D61269E}" name="Number" dataDxfId="18"/>
     <tableColumn id="2" xr3:uid="{B9AA6030-119E-443A-BB87-750EA97ECF8C}" name="Production Code Class.Method" dataDxfId="17"/>
@@ -4723,10 +4768,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16732A8-5A44-436B-B9F8-A4670902CDC5}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4992,6 +5037,210 @@
       </c>
       <c r="F16" s="12" t="s">
         <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>15</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
+        <v>16</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
+        <v>17</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="12">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="12">
+        <v>19</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="12">
+        <v>20</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
+        <v>22</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>23</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="12">
+        <v>24</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" s="12">
+        <v>25</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12">
+        <v>26</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>